<commit_message>
Updated the results for comparision with existing RPM calculator from ROBOCON 2016
</commit_message>
<xml_diff>
--- a/RPMcalculator-1.xlsx
+++ b/RPMcalculator-1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>ExpID</t>
   </si>
@@ -69,9 +69,6 @@
     <t>40Hz</t>
   </si>
   <si>
-    <t>1.1 Plot for the change in tolerance of RPM w.r.t frequency of QEI timer</t>
-  </si>
-  <si>
     <t>Y axis</t>
   </si>
   <si>
@@ -85,6 +82,21 @@
   </si>
   <si>
     <t>1.2 Plotting PWM vs RPM for QEI and Tachometer reading and observing deviation</t>
+  </si>
+  <si>
+    <t>1. Using Code Composer API</t>
+  </si>
+  <si>
+    <t>2. Using register manipulation in Kiel IDE</t>
+  </si>
+  <si>
+    <t>4Hz (Robocon 2016) frequency</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>1.1 Plot for the change in tolerance of RPM w.r.t frequency of QEI timer (Free wheel; no extenal noise)</t>
   </si>
 </sst>
 </file>
@@ -128,12 +140,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,15 +168,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>114976</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -184,8 +199,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="409575"/>
-          <a:ext cx="5105400" cy="4467901"/>
+          <a:off x="1" y="790575"/>
+          <a:ext cx="4343400" cy="3857625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>169624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>33917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8201025" y="741124"/>
+          <a:ext cx="4324350" cy="3864793"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -484,11 +543,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -496,9 +553,10 @@
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -506,67 +564,110 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F21" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Plots of PWM vs RPM (tachometer and QEI) at 10Hz and 40Hz
</commit_message>
<xml_diff>
--- a/RPMcalculator-1.xlsx
+++ b/RPMcalculator-1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>ExpID</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>1.1 Plot for the change in tolerance of RPM w.r.t frequency of QEI timer (Free wheel; no extenal noise)</t>
+  </si>
+  <si>
+    <t>(44 values averaged)</t>
+  </si>
+  <si>
+    <t>(No average)</t>
+  </si>
+  <si>
+    <t>10 HZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                               PWM vs RPM</t>
   </si>
 </sst>
 </file>
@@ -140,14 +152,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -212,15 +227,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>169624</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>7699</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>33917</xdr:rowOff>
+      <xdr:rowOff>62492</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -243,8 +258,96 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8201025" y="741124"/>
+          <a:off x="8020050" y="769699"/>
           <a:ext cx="4324350" cy="3864793"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="47625" y="9725025"/>
+          <a:ext cx="5534025" cy="4410075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>29635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6248400" y="9726085"/>
+          <a:ext cx="6038850" cy="4399490"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -543,20 +646,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="29.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,12 +670,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>19</v>
@@ -578,7 +684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -589,11 +695,11 @@
       <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
@@ -601,7 +707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>9</v>
       </c>
@@ -611,7 +717,7 @@
       <c r="H16" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -665,96 +771,164 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C28" t="s">
         <v>3</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E28" t="s">
         <v>5</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F28" t="s">
         <v>6</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>1</v>
       </c>
+      <c r="B30">
+        <v>998</v>
+      </c>
+      <c r="C30">
+        <v>23.5</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>330</v>
+      </c>
+      <c r="G30">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>500</v>
+      </c>
+      <c r="C31">
+        <v>23.5</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>290</v>
+      </c>
+      <c r="G31">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>300</v>
+      </c>
+      <c r="C32">
+        <v>23.5</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32">
+        <v>235</v>
+      </c>
+      <c r="G32">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>200</v>
+      </c>
+      <c r="C33">
+        <v>23.5</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>180</v>
+      </c>
+      <c r="G33">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>998</v>
+        <v>100</v>
       </c>
       <c r="C34">
         <v>23.5</v>
       </c>
       <c r="D34">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E34">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>85</v>
+      </c>
+      <c r="G34">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>500</v>
-      </c>
-      <c r="C35">
-        <v>23.5</v>
-      </c>
-      <c r="D35">
-        <v>40</v>
-      </c>
-      <c r="E35">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>300</v>
-      </c>
-      <c r="C36">
-        <v>23.5</v>
-      </c>
-      <c r="D36">
-        <v>40</v>
-      </c>
-      <c r="E36">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B37">
-        <v>200</v>
-      </c>
-      <c r="C37">
-        <v>23.5</v>
-      </c>
-      <c r="D37">
-        <v>40</v>
-      </c>
-      <c r="E37">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2</v>
+      </c>
       <c r="B38">
-        <v>100</v>
+        <v>998</v>
       </c>
       <c r="C38">
         <v>23.5</v>
@@ -765,49 +939,131 @@
       <c r="E38">
         <v>40</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>330.6</v>
+      </c>
+      <c r="G38">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39">
+        <v>500</v>
+      </c>
+      <c r="C39">
+        <v>23.5</v>
+      </c>
+      <c r="D39">
+        <v>40</v>
+      </c>
+      <c r="E39">
+        <v>40</v>
+      </c>
+      <c r="F39">
+        <v>290.18</v>
+      </c>
+      <c r="G39">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>300</v>
+      </c>
+      <c r="C40">
+        <v>23.5</v>
+      </c>
+      <c r="D40">
+        <v>40</v>
+      </c>
+      <c r="E40">
+        <v>40</v>
+      </c>
+      <c r="F40">
+        <v>239.386</v>
+      </c>
+      <c r="G40">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>200</v>
+      </c>
+      <c r="C41">
+        <v>23.5</v>
+      </c>
+      <c r="D41">
+        <v>40</v>
+      </c>
+      <c r="E41">
+        <v>40</v>
+      </c>
+      <c r="F41">
+        <v>181.65</v>
+      </c>
+      <c r="G41">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>100</v>
+      </c>
+      <c r="C42">
+        <v>23.5</v>
+      </c>
+      <c r="D42">
+        <v>40</v>
+      </c>
+      <c r="E42">
+        <v>40</v>
+      </c>
+      <c r="F42">
+        <v>84.5</v>
+      </c>
+      <c r="G42">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2</v>
-      </c>
-      <c r="B40">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45">
+      <c r="C43">
+        <v>23.5</v>
+      </c>
+      <c r="D43">
+        <v>40</v>
+      </c>
+      <c r="E43">
+        <v>40</v>
+      </c>
+      <c r="F43">
         <v>0</v>
       </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:XFD2"/>
-    <mergeCell ref="A31:XFD31"/>
+    <mergeCell ref="A26:XFD26"/>
+    <mergeCell ref="A46:XFD46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Conclusions of -Affect of PWM frequency on PWM vs RPM plot-
</commit_message>
<xml_diff>
--- a/RPMcalculator-1.xlsx
+++ b/RPMcalculator-1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>ExpID</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                                                                                               PWM vs RPM</t>
+  </si>
+  <si>
+    <t>1.3 Affect of PWM frequency on PWM vs RPM plot</t>
+  </si>
+  <si>
+    <t>NOTE :</t>
+  </si>
+  <si>
+    <t>* Motor heats at higher frequency due to inductance</t>
+  </si>
+  <si>
+    <t>* Screeching sound at 320KHz</t>
+  </si>
+  <si>
+    <t>* Sharper humming noise at 160KHz</t>
+  </si>
+  <si>
+    <t>* Humming noise from 80KHz PWM frequency</t>
   </si>
 </sst>
 </file>
@@ -152,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -162,6 +180,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -348,6 +369,50 @@
         <a:xfrm>
           <a:off x="6248400" y="9726085"/>
           <a:ext cx="6038850" cy="4399490"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>25814</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="14925675"/>
+          <a:ext cx="10058400" cy="5655089"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -646,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,11 +1124,42 @@
         <v>16</v>
       </c>
     </row>
+    <row r="74" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A26:XFD26"/>
     <mergeCell ref="A46:XFD46"/>
+    <mergeCell ref="A74:XFD74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Verified RPM vs PWM plots with ATMega128 controller
</commit_message>
<xml_diff>
--- a/RPMcalculator-1.xlsx
+++ b/RPMcalculator-1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>ExpID</t>
   </si>
@@ -109,24 +109,6 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                                                                                               PWM vs RPM</t>
-  </si>
-  <si>
-    <t>1.3 Affect of PWM frequency on PWM vs RPM plot</t>
-  </si>
-  <si>
-    <t>NOTE :</t>
-  </si>
-  <si>
-    <t>* Motor heats at higher frequency due to inductance</t>
-  </si>
-  <si>
-    <t>* Screeching sound at 320KHz</t>
-  </si>
-  <si>
-    <t>* Sharper humming noise at 160KHz</t>
-  </si>
-  <si>
-    <t>* Humming noise from 80KHz PWM frequency</t>
   </si>
 </sst>
 </file>
@@ -170,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -180,9 +162,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -369,50 +348,6 @@
         <a:xfrm>
           <a:off x="6248400" y="9726085"/>
           <a:ext cx="6038850" cy="4399490"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>25814</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="171450" y="14925675"/>
-          <a:ext cx="10058400" cy="5655089"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -711,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J110"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:XFD110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,42 +1059,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:1" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>33</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="A26:XFD26"/>
     <mergeCell ref="A46:XFD46"/>
-    <mergeCell ref="A74:XFD74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>